<commit_message>
1) Adjusted the Payments so they now completely follow the ethical guidelines for the experiment 2) Have completed the Test Document which now in need of commenting from Ben and Mark 3) Moved files around for the cleanliness of the repository
</commit_message>
<xml_diff>
--- a/Instructions and Documentation/Testing/Incursion, Funds, Cost Tracking and Averages 40%.xlsx
+++ b/Instructions and Documentation/Testing/Incursion, Funds, Cost Tracking and Averages 40%.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\I.T Jobs\UWA Ben White Biosecurity Project\Biosecurity Game\Instructions and Documentation\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="6DBBA894909AD11A24D3C693653414ABC8A4235E" xr6:coauthVersionLast="19" xr6:coauthVersionMax="19" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34536" windowHeight="15384" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34536" windowHeight="15384" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Incursions" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="Funds For Half 0 Half Full Cost" sheetId="9" r:id="rId7"/>
     <sheet name="Funds For Zero Costs" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171026"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,19 +34,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="45">
   <si>
-    <t>Effort Per Round</t>
+    <t>Number of Incursions</t>
   </si>
   <si>
-    <t>Game Number</t>
+    <t>Game Number - Each Game Done with 4 Participants, With the Max Protection of 15</t>
+  </si>
+  <si>
+    <t>Effort Per Round</t>
   </si>
   <si>
     <t>Random</t>
   </si>
   <si>
-    <t>Half</t>
+    <t>Quarter</t>
   </si>
   <si>
-    <t>Quarter</t>
+    <t>Half</t>
   </si>
   <si>
     <t>Three-Quarter</t>
@@ -60,19 +64,16 @@
     <t>Zero</t>
   </si>
   <si>
-    <t>Number of Incursions</t>
-  </si>
-  <si>
-    <t>Game Number - Each Game Done with 4 Participants, With the Max Protection of 15</t>
-  </si>
-  <si>
     <t>Each Game Done with 4 Participants, With the Max Protection of 15, Revenue of 25, Upkeep of 5 and kept on the Basic Biosecurity Game. The Minimum amount of Protection is $0 Which gives 40% Protection</t>
   </si>
   <si>
-    <t>Funds at Round 5</t>
+    <t>Average Number of Incursions</t>
   </si>
   <si>
-    <t>Funds at Round 15</t>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Half 0 -0 Half Full</t>
   </si>
   <si>
     <t>Player 1 Funds at Round 5 and 15</t>
@@ -87,7 +88,64 @@
     <t>Player 4 Funds at Round 5 and 15</t>
   </si>
   <si>
+    <t>Game Number</t>
+  </si>
+  <si>
+    <t>Funds at Round 5</t>
+  </si>
+  <si>
+    <t>Funds at Round 15</t>
+  </si>
+  <si>
+    <t>Game 5 Was interesting, huge variability in costs, led to interesting results, Player 3 and 4 usually contributed higher than player 1 and 2 but got better results. However there were times where Player 1 and 2 contributed higher amounts and player 3 and 4 contributed lower and lost less.</t>
+  </si>
+  <si>
+    <t>Game 7 Had Rather "Realistic" Costs by the random generator in terms of what people will probably do. Always had two players being cooperative, and one below them around $3 less and one non-cooperative, led to rather good results compared to other games.</t>
+  </si>
+  <si>
+    <t>Game 12 is a good simulation for when a group has what I'd call realistic scenario where cooperation upto round 5 was high, then after there was 1 or 2 rounds of bad luck and a breakdown in communication occurred aftergiving bad results for the group</t>
+  </si>
+  <si>
+    <t>Game 13, from observation if anyone does less than $1.50 for effort, then an incursion is rather likely to happen, however if players keep a good minimum of $6, then incursions will happen less and thus better results</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average At 5 Rounds </t>
+  </si>
+  <si>
+    <t>Average at 15 Rounds</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Player 3</t>
+  </si>
+  <si>
+    <t>Player 4</t>
+  </si>
+  <si>
     <t>Player 1-4 Funds at Round 5 and 15</t>
+  </si>
+  <si>
+    <t>Worst Case Scenario Here Game 4 - 15 Incursions</t>
+  </si>
+  <si>
+    <t>Began seeing a pattern by Game 5, Quarter amounts go one of 3 ways at this point, however, there is a good possible recovery at round 5, there is hope.</t>
+  </si>
+  <si>
+    <t>By Game 5, rather predictable in the first few rounds, what they end up with though, not predictable.</t>
+  </si>
+  <si>
+    <t>By Game 5, What I can see with this is that sometimes it can seem good to do at 3/4 max protection, but its risky! Big Rewards or Big Losses, no in between</t>
+  </si>
+  <si>
+    <t>Game 7 produced a 'nice' result, Only 4 incursions, player's fared rather well.</t>
+  </si>
+  <si>
+    <t>Game 11 showed best case scenario by round 5 for 3/4 max protection</t>
   </si>
   <si>
     <t>Player 1 and 3 Funds at Round 5 and 15</t>
@@ -99,80 +157,23 @@
     <t>Play and 4+I1:N22 Funds at Round 5 and 15</t>
   </si>
   <si>
-    <t>Game 5 Was interesting, huge variability in costs, led to interesting results, Player 3 and 4 usually contributed higher than player 1 and 2 but got better results. However there were times where Player 1 and 2 contributed higher amounts and player 3 and 4 contributed lower and lost less.</t>
-  </si>
-  <si>
-    <t>Began seeing a pattern by Game 5, Quarter amounts go one of 3 ways at this point, however, there is a good possible recovery at round 5, there is hope.</t>
-  </si>
-  <si>
-    <t>By Game 5, rather predictable in the first few rounds, what they end up with though, not predictable.</t>
-  </si>
-  <si>
-    <t>By Game 5, What I can see with this is that sometimes it can seem good to do at 3/4 max protection, but its risky! Big Rewards or Big Losses, no in between</t>
-  </si>
-  <si>
-    <t>Game 7 Had Rather "Realistic" Costs by the random generator in terms of what people will probably do. Always had two players being cooperative, and one below them around $3 less and one non-cooperative, led to rather good results compared to other games.</t>
-  </si>
-  <si>
-    <t>Worst Case Scenario Here Game 4 - 15 Incursions</t>
-  </si>
-  <si>
-    <t>Game 7 produced a 'nice' result, Only 4 incursions, player's fared rather well.</t>
-  </si>
-  <si>
     <t>Worst Case Scenario</t>
-  </si>
-  <si>
-    <t>Game 11 showed best case scenario by round 5 for 3/4 max protection</t>
-  </si>
-  <si>
-    <t>Game 12 is a good simulation for when a group has what I'd call realistic scenario where cooperation upto round 5 was high, then after there was 1 or 2 rounds of bad luck and a breakdown in communication occurred aftergiving bad results for the group</t>
-  </si>
-  <si>
-    <t>Game 13, from observation if anyone does less than $1.50 for effort, then an incursion is rather likely to happen, however if players keep a good minimum of $6, then incursions will happen less and thus better results</t>
-  </si>
-  <si>
-    <t>Average At 5 Rounds</t>
-  </si>
-  <si>
-    <t>Average at 15 Rounds</t>
   </si>
   <si>
     <t>Player 1 and 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Average At 5 Rounds </t>
-  </si>
-  <si>
     <t>Player 2 and 4</t>
   </si>
   <si>
-    <t>Player 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
-  </si>
-  <si>
-    <t>Player 3</t>
-  </si>
-  <si>
-    <t>Player 4</t>
-  </si>
-  <si>
-    <t>Average Number of Incursions</t>
-  </si>
-  <si>
-    <t>Half 0 -0 Half Full</t>
-  </si>
-  <si>
-    <t>Mode</t>
+    <t>Average At 5 Rounds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1190,24 +1191,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U356"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="15" thickBot="1">
       <c r="A1" s="6" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
@@ -1229,9 +1230,9 @@
       <c r="T1" s="8"/>
       <c r="U1" s="9"/>
     </row>
-    <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="15" thickBot="1">
       <c r="A2" s="10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="12">
         <v>1</v>
@@ -1294,9 +1295,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21">
       <c r="A3" s="11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="15">
         <v>11</v>
@@ -1359,7 +1360,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21">
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
@@ -1424,9 +1425,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21">
       <c r="A5" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" s="18">
         <v>12</v>
@@ -1489,9 +1490,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21">
       <c r="A6" s="11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="18">
         <v>5</v>
@@ -1554,9 +1555,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21">
       <c r="A7" s="11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="18">
         <v>0</v>
@@ -1619,9 +1620,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21">
       <c r="A8" s="11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="18">
         <v>14</v>
@@ -1684,9 +1685,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="15" thickBot="1">
       <c r="A9" s="21" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="22">
         <v>14</v>
@@ -1749,9 +1750,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21">
       <c r="A10" s="29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -1774,7 +1775,7 @@
       <c r="T10" s="31"/>
       <c r="U10" s="32"/>
     </row>
-    <row r="11" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" ht="15" thickBot="1">
       <c r="A11" s="30"/>
       <c r="B11" s="25"/>
       <c r="C11" s="25"/>
@@ -1797,18 +1798,18 @@
       <c r="T11" s="25"/>
       <c r="U11" s="25"/>
     </row>
-    <row r="12" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" ht="15" thickBot="1">
       <c r="A12" s="54" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B12" s="55"/>
       <c r="C12" s="55" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" s="53" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13" s="40">
         <f>AVERAGE(B3:U3)</f>
@@ -1819,7 +1820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21">
       <c r="A14" s="51" t="s">
         <v>4</v>
       </c>
@@ -1832,9 +1833,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21">
       <c r="A15" s="51" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15" s="40">
         <f t="shared" ref="B15:B19" si="1">AVERAGE(B5:U5)</f>
@@ -1845,9 +1846,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21">
       <c r="A16" s="51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="40">
         <f t="shared" si="1"/>
@@ -1858,9 +1859,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3">
       <c r="A17" s="51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B17" s="40">
         <f t="shared" si="1"/>
@@ -1871,9 +1872,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3">
       <c r="A18" s="51" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="B18" s="40">
         <f t="shared" si="1"/>
@@ -1884,9 +1885,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="15" thickBot="1">
       <c r="A19" s="52" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="56">
         <f t="shared" si="1"/>
@@ -1897,1015 +1898,1015 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="30"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3">
       <c r="A21" s="30"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3">
       <c r="A22" s="30"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3">
       <c r="A23" s="30"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3">
       <c r="A24" s="30"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3">
       <c r="A25" s="30"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3">
       <c r="A26" s="30"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3">
       <c r="A27" s="30"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3">
       <c r="A28" s="30"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3">
       <c r="A29" s="30"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3">
       <c r="A30" s="30"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3">
       <c r="A31" s="30"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3">
       <c r="A32" s="30"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1">
       <c r="A33" s="30"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1">
       <c r="A34" s="30"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1">
       <c r="A35" s="30"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1">
       <c r="A36" s="30"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1">
       <c r="A37" s="30"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1">
       <c r="A38" s="30"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1">
       <c r="A39" s="30"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1">
       <c r="A40" s="30"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1">
       <c r="A41" s="30"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1">
       <c r="A42" s="30"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1">
       <c r="A43" s="30"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1">
       <c r="A44" s="30"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1">
       <c r="A45" s="30"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:1">
       <c r="A46" s="30"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:1">
       <c r="A47" s="30"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:1">
       <c r="A48" s="30"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:1">
       <c r="A49" s="30"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:1">
       <c r="A50" s="30"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1">
       <c r="A51" s="30"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:1">
       <c r="A52" s="30"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:1">
       <c r="A53" s="30"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:1">
       <c r="A54" s="30"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:1">
       <c r="A55" s="30"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:1">
       <c r="A56" s="30"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:1">
       <c r="A57" s="30"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:1">
       <c r="A58" s="30"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:1">
       <c r="A59" s="30"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:1">
       <c r="A60" s="30"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:1">
       <c r="A61" s="30"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:1">
       <c r="A62" s="30"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:1">
       <c r="A63" s="30"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:1">
       <c r="A64" s="30"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:1">
       <c r="A65" s="30"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:1">
       <c r="A66" s="30"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:1">
       <c r="A67" s="30"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:1">
       <c r="A68" s="30"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:1">
       <c r="A69" s="30"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:1">
       <c r="A70" s="30"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:1">
       <c r="A71" s="30"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:1">
       <c r="A72" s="30"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:1">
       <c r="A73" s="30"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:1">
       <c r="A74" s="30"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:1">
       <c r="A75" s="30"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:1">
       <c r="A76" s="30"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:1">
       <c r="A77" s="30"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:1">
       <c r="A78" s="30"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:1">
       <c r="A79" s="30"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:1">
       <c r="A80" s="30"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:1">
       <c r="A81" s="30"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:1">
       <c r="A82" s="30"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:1">
       <c r="A83" s="30"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:1">
       <c r="A84" s="30"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:1">
       <c r="A85" s="30"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:1">
       <c r="A86" s="30"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:1">
       <c r="A87" s="30"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:1">
       <c r="A88" s="30"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:1">
       <c r="A89" s="30"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:1">
       <c r="A90" s="30"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:1">
       <c r="A91" s="30"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:1">
       <c r="A92" s="30"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:1">
       <c r="A93" s="30"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:1">
       <c r="A94" s="30"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:1">
       <c r="A95" s="30"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:1">
       <c r="A96" s="30"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:1">
       <c r="A97" s="30"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:1">
       <c r="A98" s="30"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:1">
       <c r="A99" s="30"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:1">
       <c r="A100" s="30"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:1">
       <c r="A101" s="30"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:1">
       <c r="A102" s="30"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:1">
       <c r="A103" s="30"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:1">
       <c r="A104" s="30"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:1">
       <c r="A105" s="30"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:1">
       <c r="A106" s="30"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:1">
       <c r="A107" s="30"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:1">
       <c r="A108" s="30"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:1">
       <c r="A109" s="30"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:1">
       <c r="A110" s="30"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:1">
       <c r="A111" s="30"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:1">
       <c r="A112" s="30"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:1">
       <c r="A113" s="30"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:1">
       <c r="A114" s="30"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:1">
       <c r="A115" s="30"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:1">
       <c r="A116" s="30"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:1">
       <c r="A117" s="30"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:1">
       <c r="A118" s="30"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:1">
       <c r="A119" s="30"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:1">
       <c r="A120" s="30"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:1">
       <c r="A121" s="30"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:1">
       <c r="A122" s="30"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:1">
       <c r="A123" s="30"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:1">
       <c r="A124" s="30"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:1">
       <c r="A125" s="30"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:1">
       <c r="A126" s="30"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:1">
       <c r="A127" s="30"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:1">
       <c r="A128" s="30"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:1">
       <c r="A129" s="30"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:1">
       <c r="A130" s="30"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:1">
       <c r="A131" s="30"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:1">
       <c r="A132" s="30"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:1">
       <c r="A133" s="30"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:1">
       <c r="A134" s="30"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:1">
       <c r="A135" s="30"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:1">
       <c r="A136" s="30"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:1">
       <c r="A137" s="30"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:1">
       <c r="A138" s="30"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:1">
       <c r="A139" s="30"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:1">
       <c r="A140" s="30"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:1">
       <c r="A141" s="30"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:1">
       <c r="A142" s="30"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:1">
       <c r="A143" s="30"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:1">
       <c r="A144" s="30"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:1">
       <c r="A145" s="30"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:1">
       <c r="A146" s="30"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:1">
       <c r="A147" s="30"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:1">
       <c r="A148" s="30"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:1">
       <c r="A149" s="30"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:1">
       <c r="A150" s="30"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:1">
       <c r="A151" s="30"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:1">
       <c r="A152" s="30"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:1">
       <c r="A153" s="30"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:1">
       <c r="A154" s="30"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:1">
       <c r="A155" s="30"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:1">
       <c r="A156" s="30"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:1">
       <c r="A157" s="30"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:1">
       <c r="A158" s="30"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:1">
       <c r="A159" s="30"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:1">
       <c r="A160" s="30"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:1">
       <c r="A161" s="30"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:1">
       <c r="A162" s="30"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:1">
       <c r="A163" s="30"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:1">
       <c r="A164" s="30"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:1">
       <c r="A165" s="30"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:1">
       <c r="A166" s="30"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:1">
       <c r="A167" s="30"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:1">
       <c r="A168" s="30"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:1">
       <c r="A169" s="30"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:1">
       <c r="A170" s="30"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:1">
       <c r="A171" s="30"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:1">
       <c r="A172" s="30"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:1">
       <c r="A173" s="30"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:1">
       <c r="A174" s="30"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:1">
       <c r="A175" s="30"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:1">
       <c r="A176" s="30"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:1">
       <c r="A177" s="30"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:1">
       <c r="A178" s="30"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:1">
       <c r="A179" s="30"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:1">
       <c r="A180" s="30"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:1">
       <c r="A181" s="30"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:1">
       <c r="A182" s="30"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:1">
       <c r="A183" s="30"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:1">
       <c r="A184" s="30"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:1">
       <c r="A185" s="30"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:1">
       <c r="A186" s="30"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:1">
       <c r="A187" s="30"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:1">
       <c r="A188" s="30"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:1">
       <c r="A189" s="30"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:1">
       <c r="A190" s="30"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:1">
       <c r="A191" s="30"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:1">
       <c r="A192" s="30"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:1">
       <c r="A193" s="30"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:1">
       <c r="A194" s="30"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:1">
       <c r="A195" s="30"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:1">
       <c r="A196" s="30"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:1">
       <c r="A197" s="30"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:1">
       <c r="A198" s="30"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:1">
       <c r="A199" s="30"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:1">
       <c r="A200" s="30"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:1">
       <c r="A201" s="30"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:1">
       <c r="A202" s="30"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:1">
       <c r="A203" s="30"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:1">
       <c r="A204" s="30"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:1">
       <c r="A205" s="30"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:1">
       <c r="A206" s="30"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:1">
       <c r="A207" s="30"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:1">
       <c r="A208" s="30"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:1">
       <c r="A209" s="30"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:1">
       <c r="A210" s="30"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:1">
       <c r="A211" s="30"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:1">
       <c r="A212" s="30"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:1">
       <c r="A213" s="30"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:1">
       <c r="A214" s="30"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:1">
       <c r="A215" s="30"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:1">
       <c r="A216" s="30"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:1">
       <c r="A217" s="30"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:1">
       <c r="A218" s="30"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:1">
       <c r="A219" s="30"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:1">
       <c r="A220" s="30"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:1">
       <c r="A221" s="30"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:1">
       <c r="A222" s="30"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:1">
       <c r="A223" s="30"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:1">
       <c r="A224" s="30"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:1">
       <c r="A225" s="30"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:1">
       <c r="A226" s="30"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:1">
       <c r="A227" s="30"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:1">
       <c r="A228" s="30"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:1">
       <c r="A229" s="30"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:1">
       <c r="A230" s="30"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:1">
       <c r="A231" s="30"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:1">
       <c r="A232" s="30"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:1">
       <c r="A233" s="30"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:1">
       <c r="A234" s="30"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:1">
       <c r="A235" s="30"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:1">
       <c r="A236" s="30"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:1">
       <c r="A237" s="30"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:1">
       <c r="A238" s="30"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:1">
       <c r="A239" s="30"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:1">
       <c r="A240" s="30"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:1">
       <c r="A241" s="30"/>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:1">
       <c r="A242" s="30"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:1">
       <c r="A243" s="30"/>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:1">
       <c r="A244" s="30"/>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:1">
       <c r="A245" s="30"/>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:1">
       <c r="A246" s="30"/>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:1">
       <c r="A247" s="30"/>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:1">
       <c r="A248" s="30"/>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:1">
       <c r="A249" s="30"/>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:1">
       <c r="A250" s="30"/>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:1">
       <c r="A251" s="30"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:1">
       <c r="A252" s="30"/>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:1">
       <c r="A253" s="30"/>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:1">
       <c r="A254" s="30"/>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:1">
       <c r="A255" s="30"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:1">
       <c r="A256" s="30"/>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:1">
       <c r="A257" s="30"/>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:1">
       <c r="A258" s="30"/>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:1">
       <c r="A259" s="30"/>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:1">
       <c r="A260" s="30"/>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:1">
       <c r="A261" s="30"/>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:1">
       <c r="A262" s="30"/>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:1">
       <c r="A263" s="30"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:1">
       <c r="A264" s="30"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:1">
       <c r="A265" s="30"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:1">
       <c r="A266" s="30"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:1">
       <c r="A267" s="30"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:1">
       <c r="A268" s="30"/>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:1">
       <c r="A269" s="30"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:1">
       <c r="A270" s="30"/>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:1">
       <c r="A271" s="30"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:1">
       <c r="A272" s="30"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:1">
       <c r="A273" s="30"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:1">
       <c r="A274" s="30"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:1">
       <c r="A275" s="30"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:1">
       <c r="A276" s="30"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:1">
       <c r="A277" s="30"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:1">
       <c r="A278" s="30"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:1">
       <c r="A279" s="30"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:1">
       <c r="A280" s="30"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:1">
       <c r="A281" s="30"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:1">
       <c r="A282" s="30"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:1">
       <c r="A283" s="30"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:1">
       <c r="A284" s="30"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:1">
       <c r="A285" s="30"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:1">
       <c r="A286" s="30"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:1">
       <c r="A287" s="30"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:1">
       <c r="A288" s="30"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:1">
       <c r="A289" s="30"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:1">
       <c r="A290" s="30"/>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:1">
       <c r="A291" s="30"/>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:1">
       <c r="A292" s="30"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:1">
       <c r="A293" s="30"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:1">
       <c r="A294" s="30"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:1">
       <c r="A295" s="30"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:1">
       <c r="A296" s="30"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:1">
       <c r="A297" s="30"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:1">
       <c r="A298" s="30"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:1">
       <c r="A299" s="30"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:1">
       <c r="A300" s="30"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:1">
       <c r="A301" s="30"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:1">
       <c r="A302" s="30"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:1">
       <c r="A303" s="30"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:1">
       <c r="A304" s="30"/>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:1">
       <c r="A305" s="30"/>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:1">
       <c r="A306" s="30"/>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:1">
       <c r="A307" s="30"/>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:1">
       <c r="A308" s="30"/>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:1">
       <c r="A309" s="30"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:1">
       <c r="A310" s="30"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:1">
       <c r="A311" s="30"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:1">
       <c r="A312" s="30"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:1">
       <c r="A313" s="30"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:1">
       <c r="A314" s="30"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:1">
       <c r="A315" s="30"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:1">
       <c r="A316" s="30"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:1">
       <c r="A317" s="30"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:1">
       <c r="A318" s="30"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:1">
       <c r="A319" s="30"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:1">
       <c r="A320" s="30"/>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:1">
       <c r="A321" s="30"/>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:1">
       <c r="A322" s="30"/>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:1">
       <c r="A323" s="30"/>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:1">
       <c r="A324" s="30"/>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:1">
       <c r="A325" s="30"/>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:1">
       <c r="A326" s="30"/>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:1">
       <c r="A327" s="30"/>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:1">
       <c r="A328" s="30"/>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:1">
       <c r="A329" s="30"/>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:1">
       <c r="A330" s="30"/>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:1">
       <c r="A331" s="30"/>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:1">
       <c r="A332" s="30"/>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:1">
       <c r="A333" s="30"/>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:1">
       <c r="A334" s="30"/>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:1">
       <c r="A335" s="30"/>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:1">
       <c r="A336" s="30"/>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:1">
       <c r="A337" s="30"/>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:1">
       <c r="A338" s="30"/>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:1">
       <c r="A339" s="30"/>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:1">
       <c r="A340" s="30"/>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:1">
       <c r="A341" s="30"/>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:1">
       <c r="A342" s="30"/>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:1">
       <c r="A343" s="30"/>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:1">
       <c r="A344" s="30"/>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:1">
       <c r="A345" s="30"/>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:1">
       <c r="A346" s="30"/>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:1">
       <c r="A347" s="30"/>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:1">
       <c r="A348" s="30"/>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:1">
       <c r="A349" s="30"/>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:1">
       <c r="A350" s="30"/>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:1">
       <c r="A351" s="30"/>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:1">
       <c r="A352" s="30"/>
     </row>
-    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:1">
       <c r="A353" s="30"/>
     </row>
-    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:1">
       <c r="A354" s="30"/>
     </row>
-    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:1">
       <c r="A355" s="30"/>
     </row>
-    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:1">
       <c r="A356" s="30"/>
     </row>
   </sheetData>
@@ -2914,29 +2915,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="69" zoomScaleNormal="69" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="11" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
@@ -2958,45 +2959,45 @@
       <c r="N1" s="36"/>
       <c r="O1" s="37"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="J2" s="34" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="K2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="M2" s="34" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="N2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="O2" s="42" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="43">
         <v>1</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>-74.42</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -3072,7 +3073,7 @@
         <v>-37.14</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -3110,7 +3111,7 @@
         <v>-18.600000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -3186,7 +3187,7 @@
         <v>34.130000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -3224,7 +3225,7 @@
         <v>-89.18</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -3262,7 +3263,7 @@
         <v>9.9700000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -3300,7 +3301,7 @@
         <v>-35.58</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>-43.99</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -3376,7 +3377,7 @@
         <v>-108.2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -3414,7 +3415,7 @@
         <v>-126.84</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -3452,7 +3453,7 @@
         <v>-69.97</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -3490,7 +3491,7 @@
         <v>36.11</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -3528,7 +3529,7 @@
         <v>-87.02</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21">
       <c r="A17" s="44">
         <v>15</v>
       </c>
@@ -3566,7 +3567,7 @@
         <v>-86.78</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21">
       <c r="A18" s="44">
         <v>16</v>
       </c>
@@ -3604,7 +3605,7 @@
         <v>-42.31</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21">
       <c r="A19" s="44">
         <v>17</v>
       </c>
@@ -3642,7 +3643,7 @@
         <v>-58.69</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="44">
         <v>18</v>
       </c>
@@ -3680,7 +3681,7 @@
         <v>-26.84</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21">
       <c r="A21" s="44">
         <v>19</v>
       </c>
@@ -3718,7 +3719,7 @@
         <v>-64.48</v>
       </c>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -3756,10 +3757,10 @@
         <v>-45.68</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1"/>
+    <row r="24" spans="1:21" ht="15" thickBot="1">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -3782,129 +3783,129 @@
       <c r="T24" s="31"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="30" spans="1:21">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15" thickBot="1"/>
+    <row r="35" spans="1:2">
+      <c r="A35" s="58" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="50"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="59" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="50"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="59" t="s">
-        <v>36</v>
       </c>
       <c r="B36" s="4">
         <f>AVERAGE(B2:B22)</f>
         <v>2.9405000000000006</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:2" ht="15" thickBot="1">
       <c r="A37" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B37" s="5">
         <f>AVERAGE(C2:C22)</f>
         <v>-45.26100000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:2" ht="15" thickBot="1">
       <c r="A38" s="57"/>
       <c r="B38" s="49"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2">
       <c r="A39" s="58" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B39" s="50"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2">
       <c r="A40" s="59" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B40" s="4">
         <f>AVERAGE(F2:F22)</f>
         <v>5.9630000000000019</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:2" ht="15" thickBot="1">
       <c r="A41" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B41" s="5">
         <f>AVERAGE(G3:G22)</f>
         <v>-40.047499999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:2" ht="15" thickBot="1">
       <c r="A42" s="57"/>
       <c r="B42" s="49"/>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2">
       <c r="A43" s="58" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B43" s="50"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2">
       <c r="A44" s="59" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B44" s="4">
         <f>AVERAGE(J2:J22)</f>
         <v>6.5745000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:2" ht="15" thickBot="1">
       <c r="A45" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B45" s="5">
         <f>AVERAGE(K3:K22)</f>
         <v>-42.076000000000008</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:2" ht="15" thickBot="1">
       <c r="A46" s="57"/>
       <c r="B46" s="49"/>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2">
       <c r="A47" s="58" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="B47" s="50"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2">
       <c r="A48" s="59" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B48" s="4">
         <f>AVERAGE(N3:N22)</f>
         <v>5.581500000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" ht="15" thickBot="1">
       <c r="A49" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B49" s="5">
         <f>AVERAGE(O3:O22)</f>
@@ -3917,31 +3918,31 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="5" max="5" width="45.77734375" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="11" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="45.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="35" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
@@ -3957,15 +3958,15 @@
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -3979,7 +3980,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" s="43">
         <v>1</v>
       </c>
@@ -4001,7 +4002,7 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -4023,7 +4024,7 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -4045,7 +4046,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -4056,7 +4057,7 @@
         <v>-106.25</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
@@ -4069,7 +4070,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -4091,7 +4092,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -4113,7 +4114,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -4135,7 +4136,7 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -4157,7 +4158,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -4179,7 +4180,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -4201,7 +4202,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -4223,7 +4224,7 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -4245,7 +4246,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -4267,7 +4268,7 @@
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -4289,7 +4290,7 @@
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21">
       <c r="A17" s="44">
         <v>15</v>
       </c>
@@ -4311,7 +4312,7 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21">
       <c r="A18" s="44">
         <v>16</v>
       </c>
@@ -4333,7 +4334,7 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21">
       <c r="A19" s="44">
         <v>17</v>
       </c>
@@ -4355,7 +4356,7 @@
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="44">
         <v>18</v>
       </c>
@@ -4377,7 +4378,7 @@
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21">
       <c r="A21" s="44">
         <v>19</v>
       </c>
@@ -4399,7 +4400,7 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -4421,10 +4422,10 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1"/>
+    <row r="24" spans="1:21" ht="15" thickBot="1">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -4447,24 +4448,24 @@
       <c r="T24" s="31"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15" thickBot="1"/>
+    <row r="32" spans="1:21">
       <c r="A32" s="58" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B32" s="50">
         <f>AVERAGE(B2:B22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="15" thickBot="1">
       <c r="A33" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B33" s="5">
         <f>AVERAGE(C2:C22)</f>
@@ -4477,31 +4478,31 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
       <selection activeCell="A32" sqref="A32:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="11" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="35" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
@@ -4517,15 +4518,15 @@
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -4539,7 +4540,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" s="43">
         <v>1</v>
       </c>
@@ -4561,7 +4562,7 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -4583,7 +4584,7 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -4605,7 +4606,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -4627,7 +4628,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -4649,7 +4650,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -4671,7 +4672,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -4693,7 +4694,7 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -4715,7 +4716,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -4737,7 +4738,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -4759,7 +4760,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -4781,7 +4782,7 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -4803,7 +4804,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -4825,7 +4826,7 @@
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -4847,7 +4848,7 @@
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21">
       <c r="A17" s="44">
         <v>15</v>
       </c>
@@ -4869,7 +4870,7 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21">
       <c r="A18" s="44">
         <v>16</v>
       </c>
@@ -4891,7 +4892,7 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21">
       <c r="A19" s="44">
         <v>17</v>
       </c>
@@ -4913,7 +4914,7 @@
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="44">
         <v>18</v>
       </c>
@@ -4935,7 +4936,7 @@
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21">
       <c r="A21" s="44">
         <v>19</v>
       </c>
@@ -4957,7 +4958,7 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -4979,10 +4980,10 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1"/>
+    <row r="24" spans="1:21" ht="15" thickBot="1">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -5005,24 +5006,24 @@
       <c r="T24" s="31"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15" thickBot="1"/>
+    <row r="32" spans="1:21">
       <c r="A32" s="58" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B32" s="50">
         <f>AVERAGE(B2:B22)</f>
         <v>6.25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="15" thickBot="1">
       <c r="A33" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B33" s="5">
         <f>AVERAGE(C2:C22)</f>
@@ -5035,31 +5036,31 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
       <selection activeCell="A32" sqref="A32:B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="11" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="35" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
@@ -5075,15 +5076,15 @@
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -5097,7 +5098,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" s="43">
         <v>1</v>
       </c>
@@ -5119,7 +5120,7 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -5141,7 +5142,7 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -5163,7 +5164,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -5185,7 +5186,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -5207,7 +5208,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -5229,7 +5230,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -5251,7 +5252,7 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -5273,7 +5274,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -5295,7 +5296,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -5317,7 +5318,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -5339,7 +5340,7 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -5361,7 +5362,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -5383,7 +5384,7 @@
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -5405,7 +5406,7 @@
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21">
       <c r="A17" s="44">
         <v>15</v>
       </c>
@@ -5427,7 +5428,7 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21">
       <c r="A18" s="44">
         <v>16</v>
       </c>
@@ -5449,7 +5450,7 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21">
       <c r="A19" s="44">
         <v>17</v>
       </c>
@@ -5471,7 +5472,7 @@
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="44">
         <v>18</v>
       </c>
@@ -5493,7 +5494,7 @@
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21">
       <c r="A21" s="44">
         <v>19</v>
       </c>
@@ -5515,7 +5516,7 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -5537,10 +5538,10 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1"/>
+    <row r="24" spans="1:21" ht="15" thickBot="1">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -5563,34 +5564,34 @@
       <c r="T24" s="31"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15" thickBot="1"/>
+    <row r="32" spans="1:21">
       <c r="A32" s="58" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B32" s="50">
         <f>AVERAGE(B2:B22)</f>
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" ht="15" thickBot="1">
       <c r="A33" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B33" s="5">
         <f>AVERAGE(C2:C22)</f>
@@ -5603,29 +5604,29 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
       <selection activeCell="A26" sqref="A26:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="11" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="35" t="s">
         <v>14</v>
       </c>
@@ -5643,15 +5644,15 @@
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -5665,7 +5666,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" s="43">
         <v>1</v>
       </c>
@@ -5687,7 +5688,7 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -5709,7 +5710,7 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -5731,7 +5732,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -5753,7 +5754,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -5775,7 +5776,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -5797,7 +5798,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -5819,7 +5820,7 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -5841,7 +5842,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -5863,7 +5864,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -5885,7 +5886,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -5907,7 +5908,7 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -5929,7 +5930,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -5951,7 +5952,7 @@
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -5973,7 +5974,7 @@
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21">
       <c r="A17" s="44">
         <v>15</v>
       </c>
@@ -5995,7 +5996,7 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21">
       <c r="A18" s="44">
         <v>16</v>
       </c>
@@ -6017,7 +6018,7 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21">
       <c r="A19" s="44">
         <v>17</v>
       </c>
@@ -6039,7 +6040,7 @@
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="44">
         <v>18</v>
       </c>
@@ -6061,7 +6062,7 @@
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21">
       <c r="A21" s="44">
         <v>19</v>
       </c>
@@ -6083,7 +6084,7 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -6105,10 +6106,10 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1"/>
+    <row r="24" spans="1:21" ht="15" thickBot="1">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -6131,19 +6132,19 @@
       <c r="T24" s="31"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="25" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="15" thickBot="1"/>
+    <row r="26" spans="1:21">
       <c r="A26" s="58" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B26" s="50">
         <f>AVERAGE(B2:B22)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="15" thickBot="1">
       <c r="A27" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5">
         <f>AVERAGE(C3:C22)</f>
@@ -6156,36 +6157,36 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:U34"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
       <selection activeCell="A32" sqref="A32:B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="11" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="35" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
       <c r="E1" s="35" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F1" s="36"/>
       <c r="G1" s="37"/>
@@ -6197,36 +6198,36 @@
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
       <c r="M2" s="46" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" s="43">
         <v>1</v>
       </c>
@@ -6253,7 +6254,7 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -6280,7 +6281,7 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -6307,7 +6308,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -6334,7 +6335,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -6361,7 +6362,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -6388,7 +6389,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -6408,7 +6409,7 @@
         <v>-50</v>
       </c>
       <c r="I9" s="48" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="J9" s="30"/>
       <c r="K9" s="30"/>
@@ -6417,7 +6418,7 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -6444,7 +6445,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -6471,7 +6472,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -6498,7 +6499,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -6525,7 +6526,7 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -6552,7 +6553,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -6579,7 +6580,7 @@
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -6606,7 +6607,7 @@
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21">
       <c r="A17" s="44">
         <v>15</v>
       </c>
@@ -6633,7 +6634,7 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21">
       <c r="A18" s="44">
         <v>16</v>
       </c>
@@ -6660,7 +6661,7 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21">
       <c r="A19" s="44">
         <v>17</v>
       </c>
@@ -6687,7 +6688,7 @@
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="44">
         <v>18</v>
       </c>
@@ -6714,7 +6715,7 @@
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21">
       <c r="A21" s="44">
         <v>19</v>
       </c>
@@ -6741,7 +6742,7 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -6768,10 +6769,10 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1"/>
+    <row r="24" spans="1:21" ht="15" thickBot="1">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -6794,50 +6795,50 @@
       <c r="T24" s="31"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="15" thickBot="1"/>
+    <row r="28" spans="1:21">
       <c r="A28" s="58" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B28" s="50"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21">
       <c r="A29" s="59" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B29" s="4">
         <f>AVERAGE(B3:B22)</f>
         <v>-52.5</v>
       </c>
     </row>
-    <row r="30" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" ht="15" thickBot="1">
       <c r="A30" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B30" s="5">
         <f>AVERAGE(C3:C22)</f>
         <v>-217.5</v>
       </c>
     </row>
-    <row r="31" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="15" thickBot="1"/>
+    <row r="32" spans="1:21">
       <c r="A32" s="58" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B32" s="50"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2">
       <c r="A33" s="59" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="B33" s="4">
         <f>AVERAGE(F3:F22)</f>
         <v>22.5</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" ht="15" thickBot="1">
       <c r="A34" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B34" s="5">
         <f>AVERAGE(G3:G22)</f>
@@ -6850,31 +6851,31 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="9" max="9" width="27.109375" customWidth="1"/>
-    <col min="10" max="11" width="18.21875" customWidth="1"/>
-    <col min="13" max="13" width="27.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" customWidth="1"/>
-    <col min="15" max="15" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.140625" customWidth="1"/>
+    <col min="10" max="11" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
+    <col min="15" max="15" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1">
       <c r="A1" s="35" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="37"/>
@@ -6890,15 +6891,15 @@
       <c r="N1" s="46"/>
       <c r="O1" s="46"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="15" thickBot="1">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E2" s="30"/>
       <c r="F2" s="30"/>
@@ -6912,7 +6913,7 @@
       <c r="N2" s="30"/>
       <c r="O2" s="30"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" s="43">
         <v>1</v>
       </c>
@@ -6934,7 +6935,7 @@
       <c r="N3" s="30"/>
       <c r="O3" s="30"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15">
       <c r="A4" s="44">
         <v>2</v>
       </c>
@@ -6956,7 +6957,7 @@
       <c r="N4" s="30"/>
       <c r="O4" s="30"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15">
       <c r="A5" s="44">
         <v>3</v>
       </c>
@@ -6978,7 +6979,7 @@
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15">
       <c r="A6" s="44">
         <v>4</v>
       </c>
@@ -7000,7 +7001,7 @@
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15">
       <c r="A7" s="44">
         <v>5</v>
       </c>
@@ -7022,7 +7023,7 @@
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15">
       <c r="A8" s="44">
         <v>6</v>
       </c>
@@ -7044,7 +7045,7 @@
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15">
       <c r="A9" s="44">
         <v>7</v>
       </c>
@@ -7066,7 +7067,7 @@
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15">
       <c r="A10" s="44">
         <v>8</v>
       </c>
@@ -7088,7 +7089,7 @@
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15">
       <c r="A11" s="44">
         <v>9</v>
       </c>
@@ -7110,7 +7111,7 @@
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" s="44">
         <v>10</v>
       </c>
@@ -7132,7 +7133,7 @@
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15">
       <c r="A13" s="44">
         <v>11</v>
       </c>
@@ -7154,7 +7155,7 @@
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15">
       <c r="A14" s="44">
         <v>12</v>
       </c>
@@ -7176,7 +7177,7 @@
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15">
       <c r="A15" s="44">
         <v>13</v>
       </c>
@@ -7198,7 +7199,7 @@
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15">
       <c r="A16" s="44">
         <v>14</v>
       </c>
@@ -7220,7 +7221,7 @@
       <c r="N16" s="30"/>
       <c r="O16" s="30"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21">
       <c r="A17" s="44">
         <v>15</v>
       </c>
@@ -7242,7 +7243,7 @@
       <c r="N17" s="30"/>
       <c r="O17" s="30"/>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21">
       <c r="A18" s="44">
         <v>16</v>
       </c>
@@ -7264,7 +7265,7 @@
       <c r="N18" s="30"/>
       <c r="O18" s="30"/>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21">
       <c r="A19" s="44">
         <v>17</v>
       </c>
@@ -7286,7 +7287,7 @@
       <c r="N19" s="30"/>
       <c r="O19" s="30"/>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21">
       <c r="A20" s="44">
         <v>18</v>
       </c>
@@ -7308,7 +7309,7 @@
       <c r="N20" s="30"/>
       <c r="O20" s="30"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21">
       <c r="A21" s="44">
         <v>19</v>
       </c>
@@ -7330,7 +7331,7 @@
       <c r="N21" s="30"/>
       <c r="O21" s="30"/>
     </row>
-    <row r="22" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" ht="15" thickBot="1">
       <c r="A22" s="45">
         <v>20</v>
       </c>
@@ -7352,10 +7353,10 @@
       <c r="N22" s="30"/>
       <c r="O22" s="30"/>
     </row>
-    <row r="23" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="24" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" ht="15" thickBot="1"/>
+    <row r="24" spans="1:21" ht="15" thickBot="1">
       <c r="A24" s="26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27"/>
@@ -7378,19 +7379,19 @@
       <c r="T24" s="31"/>
       <c r="U24" s="32"/>
     </row>
-    <row r="25" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="15" thickBot="1"/>
+    <row r="26" spans="1:21">
       <c r="A26" s="58" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B26" s="50">
         <f>AVERAGE(B3:B22)</f>
         <v>1.25</v>
       </c>
     </row>
-    <row r="27" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" ht="15" thickBot="1">
       <c r="A27" s="60" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B27" s="5">
         <f>AVERAGE(C3:C22)</f>

</xml_diff>